<commit_message>
Succeeded in addding all specimens to ImmPort, file can't contain repeats. Caught several reagent bugs while processing main, solved by providing the missing individuals as reagents. Fingers crossed
</commit_message>
<xml_diff>
--- a/ImmPort/CompletedTemplates/experimentSamples.Flow_Cytometry.xlsx
+++ b/ImmPort/CompletedTemplates/experimentSamples.Flow_Cytometry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drach\Documents\AlphaBeta\ImmPort\CompletedTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78ADCE44-54E8-4BD1-94D4-E50ED0F2F327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318F76B5-49AF-4B5A-A077-9C6103E9289D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1538,9 +1538,6 @@
     <t>ILT_01-Reference Group-DR_CXCR3 BUV737 (Cells)</t>
   </si>
   <si>
-    <t>BUV615 CD183</t>
-  </si>
-  <si>
     <t>DTR_2023_ILT_01-Reference Group-DR_CXCR3 BUV737 (Cells).fcs</t>
   </si>
   <si>
@@ -1583,27 +1580,18 @@
     <t>ILT_01-Reference Group-DR_PD1 PE-Vio770 (Cells)</t>
   </si>
   <si>
-    <t>PE-Vio770 PD1</t>
-  </si>
-  <si>
     <t>DTR_2023_ILT_01-Reference Group-DR_PD1 PE-Vio770 (Cells).fcs</t>
   </si>
   <si>
     <t>ILT_01-Reference Group-DR_TNFa PE-Dazzle594 (Cells)</t>
   </si>
   <si>
-    <t>PE-Dazzle594 TNFa</t>
-  </si>
-  <si>
     <t>DTR_2023_ILT_01-Reference Group-DR_TNFa PE-Dazzle594 (Cells).fcs</t>
   </si>
   <si>
     <t>ILT_01-Reference Group-DR_VD2 BUV661 (Cells)</t>
   </si>
   <si>
-    <t>BUV661 VD2</t>
-  </si>
-  <si>
     <t>DTR_2023_ILT_01-Reference Group-DR_VD2 BUV661 (Cells).fcs</t>
   </si>
   <si>
@@ -1620,6 +1608,18 @@
   </si>
   <si>
     <t>DTR_2023_ILT_01-Reference Group-DR_Viability_PMA Zombie NIR (Cells).fcs</t>
+  </si>
+  <si>
+    <t>BUV737 CD183</t>
+  </si>
+  <si>
+    <t>PE-Vio 770 CD279</t>
+  </si>
+  <si>
+    <t>PE-Dazzle 594 TNFa</t>
+  </si>
+  <si>
+    <t>BUV661 Vd2</t>
   </si>
 </sst>
 </file>
@@ -2104,7 +2104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B4" sqref="B4:Z66"/>
     </sheetView>
   </sheetViews>
@@ -4921,13 +4921,13 @@
         <v>240</v>
       </c>
       <c r="E57" t="s">
-        <v>383</v>
+        <v>407</v>
       </c>
       <c r="F57" t="s">
         <v>242</v>
       </c>
       <c r="G57" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="L57" t="s">
         <v>243</v>
@@ -4963,7 +4963,7 @@
     <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C58" t="s">
         <v>301</v>
@@ -4972,13 +4972,13 @@
         <v>240</v>
       </c>
       <c r="E58" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F58" t="s">
         <v>242</v>
       </c>
       <c r="G58" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="L58" t="s">
         <v>243</v>
@@ -5014,7 +5014,7 @@
     <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C59" t="s">
         <v>301</v>
@@ -5023,13 +5023,13 @@
         <v>240</v>
       </c>
       <c r="E59" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F59" t="s">
         <v>242</v>
       </c>
       <c r="G59" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="L59" t="s">
         <v>243</v>
@@ -5065,7 +5065,7 @@
     <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C60" t="s">
         <v>301</v>
@@ -5074,13 +5074,13 @@
         <v>240</v>
       </c>
       <c r="E60" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F60" t="s">
         <v>257</v>
       </c>
       <c r="G60" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="L60" t="s">
         <v>243</v>
@@ -5116,7 +5116,7 @@
     <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C61" t="s">
         <v>301</v>
@@ -5125,13 +5125,13 @@
         <v>240</v>
       </c>
       <c r="E61" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F61" t="s">
         <v>242</v>
       </c>
       <c r="G61" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L61" t="s">
         <v>243</v>
@@ -5167,7 +5167,7 @@
     <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C62" t="s">
         <v>301</v>
@@ -5176,13 +5176,13 @@
         <v>240</v>
       </c>
       <c r="E62" t="s">
-        <v>398</v>
+        <v>408</v>
       </c>
       <c r="F62" t="s">
         <v>242</v>
       </c>
       <c r="G62" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="L62" t="s">
         <v>243</v>
@@ -5218,7 +5218,7 @@
     <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C63" t="s">
         <v>301</v>
@@ -5227,13 +5227,13 @@
         <v>240</v>
       </c>
       <c r="E63" t="s">
-        <v>401</v>
+        <v>409</v>
       </c>
       <c r="F63" t="s">
         <v>257</v>
       </c>
       <c r="G63" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="L63" t="s">
         <v>243</v>
@@ -5269,7 +5269,7 @@
     <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C64" t="s">
         <v>301</v>
@@ -5278,13 +5278,13 @@
         <v>240</v>
       </c>
       <c r="E64" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
       <c r="F64" t="s">
         <v>242</v>
       </c>
       <c r="G64" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="L64" t="s">
         <v>243</v>
@@ -5320,7 +5320,7 @@
     <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="C65" t="s">
         <v>301</v>
@@ -5329,13 +5329,13 @@
         <v>240</v>
       </c>
       <c r="E65" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="F65" t="s">
         <v>242</v>
       </c>
       <c r="G65" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="L65" t="s">
         <v>243</v>
@@ -5371,7 +5371,7 @@
     <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="C66" t="s">
         <v>301</v>
@@ -5380,13 +5380,13 @@
         <v>240</v>
       </c>
       <c r="E66" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="F66" t="s">
         <v>257</v>
       </c>
       <c r="G66" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="L66" t="s">
         <v>243</v>

</xml_diff>